<commit_message>
aggiunti i dati di tutti gli esperimenti, da riguardare exp. righello
</commit_message>
<xml_diff>
--- a/Notebooks/Interferometro.xlsx
+++ b/Notebooks/Interferometro.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
-  <si>
-    <t>L focale [mm]</t>
-  </si>
-  <si>
-    <t>d [micrometri]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+  <si>
+    <t>L focale mm</t>
+  </si>
+  <si>
+    <t>d micrometri</t>
   </si>
   <si>
     <t>n frange</t>
@@ -28,10 +28,19 @@
     <t xml:space="preserve">raggio </t>
   </si>
   <si>
-    <t>Deltad eff [microm]</t>
-  </si>
-  <si>
-    <t>DeltaN</t>
+    <t>costheta</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Deltad eff fp</t>
+  </si>
+  <si>
+    <t>DeltaN fp</t>
   </si>
   <si>
     <t>DeltaN medio</t>
@@ -40,10 +49,61 @@
     <t>Michelson</t>
   </si>
   <si>
-    <t>d(lente,schermo) [cm]</t>
-  </si>
-  <si>
-    <t>lamda [microm]</t>
+    <t>Deltad eff m</t>
+  </si>
+  <si>
+    <t>DeltaN m</t>
+  </si>
+  <si>
+    <t>medio</t>
+  </si>
+  <si>
+    <t>Vetro</t>
+  </si>
+  <si>
+    <t>theta i</t>
+  </si>
+  <si>
+    <t>theta f</t>
+  </si>
+  <si>
+    <t>deltaN v</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>Righello</t>
+  </si>
+  <si>
+    <t>dPt,P0</t>
+  </si>
+  <si>
+    <t>dP0,Pi</t>
+  </si>
+  <si>
+    <t>costheta inc</t>
+  </si>
+  <si>
+    <t>costheta N</t>
+  </si>
+  <si>
+    <t>d(lente,schermo) cm</t>
+  </si>
+  <si>
+    <t>dsorgente,schermo</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>lamda microm</t>
+  </si>
+  <si>
+    <t>dlaser,righello</t>
+  </si>
+  <si>
+    <t>spessore vetro mm</t>
   </si>
 </sst>
 </file>
@@ -116,14 +176,14 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,7 +487,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -435,18 +495,37 @@
   <cols>
     <col min="1" max="1" style="7" width="20.433571428571426" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="11.005" customWidth="1" bestFit="1"/>
     <col min="12" max="12" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="19.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="7" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="10" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="10" width="11.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -465,31 +544,78 @@
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>5</v>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B2" s="6">
         <v>160.5</v>
@@ -503,33 +629,84 @@
       <c r="E2" s="6">
         <v>3.7</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="6">
+        <f>$B$2/SQRT($B$2^2+E2^2)</f>
+      </c>
       <c r="G2" s="2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2">
+        <f>F2-$F$2</f>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2">
         <v>10</v>
       </c>
-      <c r="H2" s="2">
+      <c r="L2" s="2">
         <v>27</v>
       </c>
-      <c r="I2" s="6">
-        <f>average(H2:H6)</f>
-      </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="6">
+      <c r="M2" s="6">
+        <f>AVERAGE(L2:L6)</f>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="6">
         <v>167.8</v>
       </c>
-      <c r="M2" s="2">
+      <c r="Q2" s="2">
         <v>10</v>
       </c>
-      <c r="N2" s="2">
+      <c r="R2" s="2">
         <v>29</v>
+      </c>
+      <c r="S2" s="2">
+        <f>AVERAGE(R2:R6)</f>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="2">
+        <f>219-53</f>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="6">
+        <v>2</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z2" s="6">
+        <f>AVERAGE(Y2:Y6)</f>
+      </c>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>129</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>13.8</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>1.4</v>
+      </c>
+      <c r="AF2" s="6">
+        <f>AC2/SQRT((AD2/2)^2+AC2^2)</f>
+      </c>
+      <c r="AG2" s="6">
+        <f>$AC$2/SQRT($AC$2^2+(($AD$2/2)+AE2)^2)</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6">
         <v>0.6328</v>
@@ -539,89 +716,217 @@
       <c r="E3" s="6">
         <v>3.3</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="2">
+      <c r="F3" s="6">
+        <f>$B$2/SQRT($B$2^2+E3^2)</f>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <f>F3-$F$2</f>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="2">
         <v>32</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="2">
+      <c r="M3" s="5"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="2">
         <v>33</v>
       </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC3" s="2">
+        <v>229</v>
+      </c>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="6">
+        <f>$AC$2/SQRT($AC$2^2+(($AD$2/2)+AE3)^2)</f>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="6">
         <v>2.9</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2">
+      <c r="F4" s="6">
+        <f>$B$2/SQRT($B$2^2+E4^2)</f>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6">
+        <f>F4-$F$2</f>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="2">
         <v>29</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="2">
+      <c r="M4" s="5"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="2">
         <v>28</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="6">
+        <v>3.6</v>
+      </c>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="6">
+        <f>$AC$2/SQRT($AC$2^2+(($AD$2/2)+AE4)^2)</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="6">
         <v>2.2</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2">
+      <c r="F5" s="6">
+        <f>$B$2/SQRT($B$2^2+E5^2)</f>
+      </c>
+      <c r="G5" s="2">
+        <v>3</v>
+      </c>
+      <c r="H5" s="6">
+        <f>F5-$F$2</f>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2">
         <v>30</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="2">
+      <c r="M5" s="5"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="2">
         <v>29</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="2">
+        <v>6</v>
+      </c>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="6">
+        <v>4.6</v>
+      </c>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="6">
+        <f>$AC$2/SQRT($AC$2^2+(($AD$2/2)+AE5)^2)</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1"/>
-      <c r="B6" s="5"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="6">
         <v>1.35</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2">
+      <c r="F6" s="6">
+        <f>$B$2/SQRT($B$2^2+E6^2)</f>
+      </c>
+      <c r="G6" s="2">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6">
+        <f>F6-$F$2</f>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="2">
         <v>29</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="2">
+      <c r="M6" s="5"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="2">
         <v>31</v>
       </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="2">
+        <v>7</v>
+      </c>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1"/>
-      <c r="B7" s="5"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="2">
         <v>46</v>
       </c>
@@ -629,117 +934,248 @@
       <c r="E7" s="6">
         <v>3.7</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="2">
+      <c r="F7" s="6">
+        <f>$B$2/SQRT($B$2^2+E7^2)</f>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="2">
+        <f>F7-$F$7</f>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="2">
         <v>7</v>
       </c>
-      <c r="H7" s="2">
+      <c r="L7" s="2">
         <v>19</v>
       </c>
-      <c r="I7" s="6">
-        <f>average(H7:H11)</f>
-      </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="2">
+      <c r="M7" s="6">
+        <f>AVERAGE(L7:L11)</f>
+      </c>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="2">
         <v>7</v>
       </c>
-      <c r="N7" s="2">
+      <c r="R7" s="2">
         <v>22</v>
       </c>
+      <c r="S7" s="6">
+        <f>AVERAGE(R7:R11)</f>
+      </c>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="6">
+        <v>3</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>21</v>
+      </c>
+      <c r="Z7" s="6">
+        <f>AVERAGE(Y7:Y11)</f>
+      </c>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="5"/>
+      <c r="AE7" s="5"/>
+      <c r="AF7" s="5"/>
+      <c r="AG7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="6">
         <v>3.3</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="6">
+        <f>$B$2/SQRT($B$2^2+E8^2)</f>
+      </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="2">
+      <c r="H8" s="6">
+        <f>F8-$F$7</f>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="2">
         <v>22</v>
       </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="2">
+      <c r="M8" s="5"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="2">
         <v>21</v>
       </c>
+      <c r="S8" s="5"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="2">
+        <v>22</v>
+      </c>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="5"/>
+      <c r="AE8" s="5"/>
+      <c r="AF8" s="5"/>
+      <c r="AG8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="6">
         <v>2.9</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="6">
+        <f>$B$2/SQRT($B$2^2+E9^2)</f>
+      </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="2">
+      <c r="H9" s="6">
+        <f>F9-$F$7</f>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="2">
         <v>20</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="2">
+      <c r="M9" s="5"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="2">
         <v>18</v>
       </c>
+      <c r="S9" s="5"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="2">
+        <v>21</v>
+      </c>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="5"/>
+      <c r="AE9" s="5"/>
+      <c r="AF9" s="5"/>
+      <c r="AG9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="6">
         <v>2.25</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="6">
+        <f>$B$2/SQRT($B$2^2+E10^2)</f>
+      </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="2">
+      <c r="H10" s="6">
+        <f>F10-$F$7</f>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="2">
         <v>20</v>
       </c>
-      <c r="I10" s="5"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="2">
+      <c r="M10" s="5"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="2">
         <v>21</v>
       </c>
+      <c r="S10" s="5"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="2">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="5"/>
+      <c r="AE10" s="5"/>
+      <c r="AF10" s="5"/>
+      <c r="AG10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="6">
         <v>1.4</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="6">
+        <f>$B$2/SQRT($B$2^2+E11^2)</f>
+      </c>
       <c r="G11" s="3"/>
-      <c r="H11" s="2">
+      <c r="H11" s="6">
+        <f>F11-$F$7</f>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="2">
         <v>21</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="2">
+      <c r="M11" s="5"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="2">
         <v>20</v>
       </c>
+      <c r="S11" s="5"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="2">
+        <v>22</v>
+      </c>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="5"/>
+      <c r="AE11" s="5"/>
+      <c r="AF11" s="5"/>
+      <c r="AG11" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="2">
         <v>65</v>
       </c>
@@ -747,117 +1183,248 @@
       <c r="E12" s="6">
         <v>3.7</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="2">
+      <c r="F12" s="6">
+        <f>$B$2/SQRT($B$2^2+E12^2)</f>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2">
+        <f>F12-$F$2</f>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2">
         <v>5</v>
       </c>
-      <c r="H12" s="2">
+      <c r="L12" s="2">
         <v>15</v>
       </c>
-      <c r="I12" s="6">
-        <f>average(H12:H16)</f>
-      </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="2">
+      <c r="M12" s="6">
+        <f>AVERAGE(L12:L16)</f>
+      </c>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="2">
         <v>5</v>
       </c>
-      <c r="N12" s="2">
+      <c r="R12" s="2">
         <v>14</v>
       </c>
+      <c r="S12" s="6">
+        <f>AVERAGE(R12:R16)</f>
+      </c>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="6">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="6">
+        <f>AVERAGE(Y12:Y16)</f>
+      </c>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="5"/>
+      <c r="AE12" s="5"/>
+      <c r="AF12" s="5"/>
+      <c r="AG12" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="6">
         <v>3.2</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="6">
+        <f>$B$2/SQRT($B$2^2+E13^2)</f>
+      </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="2">
+      <c r="H13" s="6">
+        <f>F18-$F$2</f>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="2">
         <v>14</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="2">
+      <c r="M13" s="5"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="2">
         <v>15</v>
       </c>
+      <c r="S13" s="5"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="3"/>
+      <c r="W13" s="3"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="5"/>
+      <c r="AE13" s="5"/>
+      <c r="AF13" s="5"/>
+      <c r="AG13" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="6">
         <v>2.7</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="6">
+        <f>$B$2/SQRT($B$2^2+E14^2)</f>
+      </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="2">
+      <c r="H14" s="6">
+        <f>F19-$F$2</f>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="2">
         <v>14</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="2">
+      <c r="M14" s="5"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="2">
         <v>17</v>
       </c>
+      <c r="S14" s="5"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="5"/>
+      <c r="AE14" s="5"/>
+      <c r="AF14" s="5"/>
+      <c r="AG14" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="6">
         <v>2.1</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="6">
+        <f>$B$2/SQRT($B$2^2+E15^2)</f>
+      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="2">
+      <c r="H15" s="6">
+        <f>F20-$F$2</f>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="2">
         <v>14</v>
       </c>
-      <c r="I15" s="5"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="2">
+      <c r="M15" s="5"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="2">
         <v>15</v>
       </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="5"/>
+      <c r="AE15" s="5"/>
+      <c r="AF15" s="5"/>
+      <c r="AG15" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="6">
         <v>1.1</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="6">
+        <f>$B$2/SQRT($B$2^2+E16^2)</f>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="2">
+      <c r="H16" s="6">
+        <f>F21-$F$2</f>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="2">
         <v>16</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="2">
+      <c r="M16" s="5"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2">
         <v>16</v>
       </c>
+      <c r="S16" s="5"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="5"/>
+      <c r="AE16" s="5"/>
+      <c r="AF16" s="5"/>
+      <c r="AG16" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="2">
         <v>81</v>
       </c>
@@ -865,91 +1432,206 @@
       <c r="E17" s="6">
         <v>3.7</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="6">
+        <f>$B$2/SQRT($B$2^2+E17^2)</f>
+      </c>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="5"/>
+      <c r="H17" s="2">
+        <f>F22-$F$2</f>
+      </c>
+      <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="5"/>
+      <c r="AE17" s="5"/>
+      <c r="AF17" s="5"/>
+      <c r="AG17" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="6">
         <v>3.3</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="6">
+        <f>$B$2/SQRT($B$2^2+E18^2)</f>
+      </c>
       <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="5"/>
+      <c r="H18" s="6">
+        <f>F23-$F$2</f>
+      </c>
+      <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="5"/>
+      <c r="AF18" s="5"/>
+      <c r="AG18" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="6">
         <v>2.8</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="6">
+        <f>$B$2/SQRT($B$2^2+E19^2)</f>
+      </c>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="5"/>
+      <c r="H19" s="6">
+        <f>F24-$F$2</f>
+      </c>
+      <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="5"/>
+      <c r="AE19" s="5"/>
+      <c r="AF19" s="5"/>
+      <c r="AG19" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="6">
         <v>2.1</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="6">
+        <f>$B$2/SQRT($B$2^2+E20^2)</f>
+      </c>
       <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="5"/>
+      <c r="H20" s="6">
+        <f>F25-$F$2</f>
+      </c>
+      <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="6">
         <v>1.3</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="6">
+        <f>$B$2/SQRT($B$2^2+E21^2)</f>
+      </c>
       <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="5"/>
+      <c r="H21" s="6">
+        <f>F26-$F$2</f>
+      </c>
+      <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="2">
         <v>96</v>
       </c>
@@ -957,91 +1639,206 @@
       <c r="E22" s="6">
         <v>3.7</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="6">
+        <f>$B$2/SQRT($B$2^2+E22^2)</f>
+      </c>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
+      <c r="H22" s="2">
+        <f>F27-$F$2</f>
+      </c>
+      <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="3"/>
+      <c r="W22" s="3"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="3"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="6">
         <v>3.3</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="6">
+        <f>$B$2/SQRT($B$2^2+E23^2)</f>
+      </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="5"/>
+      <c r="H23" s="6">
+        <f>F28-$F$2</f>
+      </c>
+      <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="5"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="6">
         <v>2.8</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="6">
+        <f>$B$2/SQRT($B$2^2+E24^2)</f>
+      </c>
       <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="5"/>
+      <c r="H24" s="6">
+        <f>F29-$F$2</f>
+      </c>
+      <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AG24" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="6">
         <v>2.1</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="6">
+        <f>$B$2/SQRT($B$2^2+E25^2)</f>
+      </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="5"/>
+      <c r="H25" s="6">
+        <f>F30-$F$2</f>
+      </c>
+      <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="6">
         <v>1.3</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="6">
+        <f>$B$2/SQRT($B$2^2+E26^2)</f>
+      </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="5"/>
+      <c r="H26" s="6">
+        <f>F31-$F$2</f>
+      </c>
+      <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="3"/>
       <c r="C27" s="2">
         <v>110</v>
       </c>
@@ -1049,87 +1846,202 @@
       <c r="E27" s="6">
         <v>3.7</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="6">
+        <f>$B$2/SQRT($B$2^2+E27^2)</f>
+      </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="5"/>
+      <c r="H27" s="2">
+        <f>F32-$F$2</f>
+      </c>
+      <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
-      <c r="B28" s="5"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="6">
         <v>3.3</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="6">
+        <f>$B$2/SQRT($B$2^2+E28^2)</f>
+      </c>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="5"/>
+      <c r="H28" s="6">
+        <f>F33-$F$2</f>
+      </c>
+      <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="6">
         <v>2.8</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="6">
+        <f>$B$2/SQRT($B$2^2+E29^2)</f>
+      </c>
       <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="5"/>
+      <c r="H29" s="6">
+        <f>F34-$F$2</f>
+      </c>
+      <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="5"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="6">
         <v>2.2</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="6">
+        <f>$B$2/SQRT($B$2^2+E30^2)</f>
+      </c>
       <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="5"/>
+      <c r="H30" s="6">
+        <f>F35-$F$2</f>
+      </c>
+      <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="5"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="6">
         <v>1.35</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="6">
+        <f>$B$2/SQRT($B$2^2+E31^2)</f>
+      </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="5"/>
+      <c r="H31" s="6">
+        <f>F36-$F$2</f>
+      </c>
+      <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>